<commit_message>
update gpu workstation configuration
</commit_message>
<xml_diff>
--- a/data/deep-learning-server.xlsx
+++ b/data/deep-learning-server.xlsx
@@ -8,15 +8,24 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\swc\united_states\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{187C2110-A1DB-40B0-883F-AFA284FC4BD5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFDDE0A1-4C5F-4796-8396-34EA8D57C7EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" activeTab="3" xr2:uid="{65FE6386-AB1C-4CB3-ACD7-B24F3EF59184}"/>
+    <workbookView xWindow="-24690" yWindow="870" windowWidth="19755" windowHeight="12105" firstSheet="1" activeTab="6" xr2:uid="{65FE6386-AB1C-4CB3-ACD7-B24F3EF59184}"/>
   </bookViews>
   <sheets>
-    <sheet name="GPU" sheetId="1" r:id="rId1"/>
-    <sheet name="Memory" sheetId="2" r:id="rId2"/>
-    <sheet name="cpu" sheetId="3" r:id="rId3"/>
-    <sheet name="ssd" sheetId="4" r:id="rId4"/>
+    <sheet name="amd_intel" sheetId="13" r:id="rId1"/>
+    <sheet name="GPU" sheetId="1" r:id="rId2"/>
+    <sheet name="Memory" sheetId="2" r:id="rId3"/>
+    <sheet name="cpu" sheetId="3" r:id="rId4"/>
+    <sheet name="ssd" sheetId="4" r:id="rId5"/>
+    <sheet name="--" sheetId="5" r:id="rId6"/>
+    <sheet name="server" sheetId="6" r:id="rId7"/>
+    <sheet name="아싸" sheetId="7" r:id="rId8"/>
+    <sheet name="ITmaya" sheetId="8" r:id="rId9"/>
+    <sheet name="---" sheetId="9" r:id="rId10"/>
+    <sheet name="202108" sheetId="10" r:id="rId11"/>
+    <sheet name="202205" sheetId="11" r:id="rId12"/>
+    <sheet name="202011" sheetId="12" r:id="rId13"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="263" uniqueCount="197">
   <si>
     <t>GPU</t>
   </si>
@@ -183,16 +192,532 @@
   </si>
   <si>
     <t>https://diskprices.com/?locale=us&amp;condition=new&amp;disk_types=external_ssd,internal_ssd,m2_ssd,m2_nvme,u2</t>
+  </si>
+  <si>
+    <t>품명</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>제품사양</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>수량</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>CASE</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>CORSAIR OBSISIAN 750D AIRFLOWER</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>CPU</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">인텔 코어X I9 10980XE  캐스케이드레이크 </t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>쿨러</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>NZXT KRAKEN X63 ( 3열수랭)</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>RAM</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>M/B</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>VGA</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>SSD</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>삼성 980 PRO M.2 NVMe 1TB</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>HDD</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>WD RED 4TB</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>POWER</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>EVGA SUPERNOVA 2000G+ 80PLUS GOLD</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>단가</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>가격</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>NVIDIA 지포스 갤럭시 RTX 3090 SG D6X 24GB</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">삼성 DDR4-2933 32GB </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="마루 부리 중간"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t xml:space="preserve"> (총 256GB )</t>
+    </r>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>누적비율</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>비율</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>순</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>===============================================================================</t>
+  </si>
+  <si>
+    <t>■ 제품수량 : 1대 / 견적합계 : 7,505,210원 (VAT포함)</t>
+  </si>
+  <si>
+    <t>■ 제품명 : 딥러닝 SV2</t>
+  </si>
+  <si>
+    <t>[삼성] 1TB SSD[NVMe/TLC/D램/PM9A1]</t>
+  </si>
+  <si>
+    <t>제품 저장 : https://www.assacom.com/shop/product/auto_make_system/mWVnaGmYnw%3D%3D</t>
+  </si>
+  <si>
+    <t>부품</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>부품상세</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>[인텔] 16코어 엘더 i9 12900K 터보5.2G</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>[아수스] Z690-E 게이밍WIFI[D5/HDMI/DP]</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>[삼성/PNC] 32G 4800MHz[16G×2]리모콘/RGB</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>[아수스] 지포스 RTX3090[24GB/OC] X 2개</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>단가</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>수량</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>총가격</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>[에너맥스] 리큐맥스 III ARGB 360 [360]</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>[EVGA] 2000W 정격 APFC[80+골드]</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>[쓰리알] 빅타워[T840 풍통 블랙]</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>그래픽VGA</t>
+  </si>
+  <si>
+    <t>CPU</t>
+  </si>
+  <si>
+    <t>메인보드</t>
+  </si>
+  <si>
+    <t>파워</t>
+  </si>
+  <si>
+    <t>메모리RAM</t>
+  </si>
+  <si>
+    <t>쿨러</t>
+  </si>
+  <si>
+    <t>저장소SSD</t>
+  </si>
+  <si>
+    <t>케이스</t>
+  </si>
+  <si>
+    <t>2GPU x NVIDIA RTX3090</t>
+  </si>
+  <si>
+    <t> 64GB (32GB x2) DDR4 ECC-RDIMM 2933 Memory</t>
+  </si>
+  <si>
+    <t>1CPU x Intel Xeon W-2235 6C/12T</t>
+  </si>
+  <si>
+    <t>단종</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>1300W 80PLUS Platinum Single Power</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">CPU </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> [삼성전자] 삼성 DDR4 16GB PC4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SSD </t>
+  </si>
+  <si>
+    <t xml:space="preserve">케이스 </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> [마이크로닉스] Classic II 1050W 80PLUS GOLD 230V EU 풀모듈러 (ATX/1050W)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CPU 쿨러 </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> [THERMOLAB] TRINITY 6.0 [CPU쿨러]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">그래픽카드 </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 이엠텍 지포스 RTX 3060 STORM X Dual OC D6 12GB</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> [BRAVOTEC] 스텔스 EX270 파노라마 윈도우 블랙(빅타워) </t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>파워서플라이</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> [삼성전자] 공식인증 980 series 500GB M.2 NVMe 500GB MZ - V8V500BW</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve"> [INTEL] 코어11세대 i5 11400</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>RAM</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve"> [ASUS] ROG STRIX Z590-E GAMING WIFI RAM</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">메인보드 </t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>2021년 8월 기준 200만원</t>
+  </si>
+  <si>
+    <t>https://taptorestart.tistory.com/entry/%EB%94%A5%EB%9F%AC%EB%8B%9DDeep-Learning-%EA%B3%B5%EB%B6%80%EB%A5%BC-%EC%9C%84%ED%95%9C-%EC%84%9C%EB%B2%84%EC%9A%A9-%EB%8D%B0%EC%8A%A4%ED%81%AC%ED%83%91-%EC%BB%B4%ED%93%A8%ED%84%B0-%EA%B5%AC%EC%9E%85%EA%B8%B0</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>출처: https://ckdals29672.tistory.com/3?category=976842 [후드 쓴 아이의 개발일지:티스토리]</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> galaxy RTX 3090 sg, </t>
+  </si>
+  <si>
+    <t>SSD</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Antec NeoECO 850W 80PLUS GOLD, </t>
+  </si>
+  <si>
+    <t>시스템 쿨러</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ARCTIC P14 PWM x2, </t>
+  </si>
+  <si>
+    <t>CPU쿨러</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 잘만 CNPS10X performa black, </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> NZXT h510 flow</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> i7-12700, </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> asus-tuf gaming z690-plus, </t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve"> 삼성 970 evo plus 1TB, sk 하이닉스 Gold 500GB, </t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://m.blog.naver.com/hanwoo10303/222139462201</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>i9 10980XE</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>기가바이트 x299 wu8</t>
+  </si>
+  <si>
+    <t>삼성 DDR4 32G</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>삼성전자 970 PRO M.2 NVMe 1TB</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>지포스 RTX 3090 슈프림 X D6X 24GB</t>
+  </si>
+  <si>
+    <t>SuperFlower SF-2000F14HP LEADEX PLATINUM</t>
+  </si>
+  <si>
+    <t>ASUS PRIME X299 SAGE STCOM</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>Year</t>
+  </si>
+  <si>
+    <t>Intel Model</t>
+  </si>
+  <si>
+    <t>AMD Model</t>
+  </si>
+  <si>
+    <t>Notes</t>
+  </si>
+  <si>
+    <t>Pentium 4 2.0GHz (1c/1t)</t>
+  </si>
+  <si>
+    <t>Athlon XP 1900+ (1c/1t)</t>
+  </si>
+  <si>
+    <t>Pentium 4 2.8GHz (1c/2t)</t>
+  </si>
+  <si>
+    <t>Athlon XP 2800+ (1c/1t)</t>
+  </si>
+  <si>
+    <t>Intel introduces hyperthreading</t>
+  </si>
+  <si>
+    <t>Pentium 4 Extreme 3.2GHz (1c/2t)</t>
+  </si>
+  <si>
+    <t>Athlon XP 3200+ (1c/1t)</t>
+  </si>
+  <si>
+    <t>Pentium 4 3.4GHz (1c/2t)</t>
+  </si>
+  <si>
+    <t>Athlon 64 FX-55 (1c/1t)</t>
+  </si>
+  <si>
+    <t>Pentium 4 3.8GHz (1c/2t)</t>
+  </si>
+  <si>
+    <t>Athlon 64 X2 4800+ (2c/2t)</t>
+  </si>
+  <si>
+    <t>Pentium Extreme 965 (2c/4t)</t>
+  </si>
+  <si>
+    <t>Athlon 64 X2 5000+ (2c/2t)</t>
+  </si>
+  <si>
+    <t>Intel takes the undisputed performance lead here—and keeps it for a decade straight.</t>
+  </si>
+  <si>
+    <t>Core 2 Extreme QX6800 (4c/4t)</t>
+  </si>
+  <si>
+    <t>Phenom X4 9600 (4c/4t)</t>
+  </si>
+  <si>
+    <t>Intel and AMD both launch the first true quad-core desktop CPUs</t>
+  </si>
+  <si>
+    <t>Core 2 Extreme X9650 (4c/4t)</t>
+  </si>
+  <si>
+    <t>Phenom X4 9950 (4c/4t)</t>
+  </si>
+  <si>
+    <t>Core i7-960 (4c/8t)</t>
+  </si>
+  <si>
+    <t>Phenom II X4 965 (4c/4t)</t>
+  </si>
+  <si>
+    <t>Core i7-980X (6c/12t)</t>
+  </si>
+  <si>
+    <t>Phenom II X6 1100T (6c/6t)</t>
+  </si>
+  <si>
+    <t>Intel and AMD both introduce hex-core desktop CPUs</t>
+  </si>
+  <si>
+    <t>Core i7-990X (6c/12t)</t>
+  </si>
+  <si>
+    <t>FX-8150 (8c/8t)</t>
+  </si>
+  <si>
+    <t>Core i7-3770K (4c/8t)</t>
+  </si>
+  <si>
+    <t>FX-8350 (8c/8t)</t>
+  </si>
+  <si>
+    <t>Intel abandons hex-core desktop CPUs—but few miss them, due to large single-threaded gains</t>
+  </si>
+  <si>
+    <t>Core i7-4770K (4c/8t)</t>
+  </si>
+  <si>
+    <t>FX-9590 (8c/8t)</t>
+  </si>
+  <si>
+    <t>AMD's underwhelming FX-9590 launches—and it's Team Red's last enthusiast CPU for four long years</t>
+  </si>
+  <si>
+    <t>Core i7-4790K (4c/8t)</t>
+  </si>
+  <si>
+    <t>Intel's 5th generation Core dies stillborn. AMD releases low-power APUs, but no successor to FX-9590</t>
+  </si>
+  <si>
+    <t>Core i7-6700K (4c/8t)</t>
+  </si>
+  <si>
+    <t>Core i7-7700K (4c/8t)</t>
+  </si>
+  <si>
+    <t>Strictly speaking, 2016 was an Intel whiff—Kaby Lake didn't actually launch until January 2017</t>
+  </si>
+  <si>
+    <t>Core i7-8700K (6c/12t)</t>
+  </si>
+  <si>
+    <t>Ryzen 7 1800X (8c/16t)</t>
+  </si>
+  <si>
+    <t>Launch of AMD's Zen architecture, return of the Intel hex-core desktop CPU</t>
+  </si>
+  <si>
+    <t>Core i9-9900K (8c/16t)</t>
+  </si>
+  <si>
+    <t>Ryzen 7 2700X (8c/16t)</t>
+  </si>
+  <si>
+    <t>Core i9-9900KS (8c/16t)</t>
+  </si>
+  <si>
+    <t>Ryzen 9 3950X (16c/32t)</t>
+  </si>
+  <si>
+    <t>AMD's Zen 2 architecture launches, Intel whiffs hard in the performance segment</t>
+  </si>
+  <si>
+    <t>Core i9-10900K (10c/20t)</t>
+  </si>
+  <si>
+    <t>Ryzen 9 5950X (16c/32t)</t>
+  </si>
+  <si>
+    <t>AMD's Zen 3 finally crushes Intel's long-held single-threaded performance record</t>
+  </si>
+  <si>
+    <t>구분</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>워크스테이션</t>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="4">
+    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="24" formatCode="\$#,##0_);[Red]\(\$#,##0\)"/>
+    <numFmt numFmtId="176" formatCode="#,##0_ "/>
+    <numFmt numFmtId="177" formatCode="0.0%"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="15">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -229,8 +754,81 @@
       <charset val="129"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="맑은 고딕"/>
+      <family val="2"/>
+      <charset val="129"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="돋움"/>
+      <family val="3"/>
+      <charset val="129"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <name val="마루 부리 중간"/>
+      <family val="3"/>
+      <charset val="129"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="마루 부리 중간"/>
+      <family val="3"/>
+      <charset val="129"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <name val="마루 부리 중간"/>
+      <family val="3"/>
+      <charset val="129"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FFFF0000"/>
+      <name val="마루 부리 중간"/>
+      <family val="3"/>
+      <charset val="129"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="맑은 고딕"/>
+      <family val="3"/>
+      <charset val="129"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FF333333"/>
+      <name val="돋움"/>
+      <family val="3"/>
+      <charset val="129"/>
+    </font>
+    <font>
+      <sz val="6"/>
+      <color rgb="FF000000"/>
+      <name val="Opensans"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="6"/>
+      <color rgb="FF000000"/>
+      <name val="Opensans"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -255,8 +853,38 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-4.9989318521683403E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF0F1F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF6F6F6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="14">
     <border>
       <left/>
       <right/>
@@ -273,16 +901,188 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="dashed">
+        <color indexed="64"/>
+      </top>
+      <bottom style="dashed">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="dashed">
+        <color indexed="64"/>
+      </top>
+      <bottom style="dashed">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="dashed">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="dashed">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="dashed">
+        <color indexed="64"/>
+      </top>
+      <bottom style="dashed">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color rgb="FF839496"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color rgb="FF839496"/>
+      </top>
+      <bottom style="thick">
+        <color rgb="FFDDDDDD"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="41" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -340,8 +1140,118 @@
     <xf numFmtId="10" fontId="1" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="9" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="9" fillId="0" borderId="8" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="9" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="176" fontId="9" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="11" xfId="2" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="11" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="11" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="9" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="8" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="4">
+    <cellStyle name="백분율" xfId="3" builtinId="5"/>
+    <cellStyle name="쉼표 [0]" xfId="2" builtinId="6"/>
     <cellStyle name="표준" xfId="0" builtinId="0"/>
     <cellStyle name="하이퍼링크" xfId="1" builtinId="8"/>
   </cellStyles>
@@ -654,6 +1564,1053 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3EA52933-0D71-4D35-98A3-D6CFA29BA4B7}">
+  <dimension ref="A1:D22"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E18" sqref="E18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="41" defaultRowHeight="17"/>
+  <cols>
+    <col min="1" max="1" width="3.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.58203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="39.83203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="17.5" thickBot="1">
+      <c r="A1" s="51" t="s">
+        <v>143</v>
+      </c>
+      <c r="B1" s="51" t="s">
+        <v>144</v>
+      </c>
+      <c r="C1" s="51" t="s">
+        <v>145</v>
+      </c>
+      <c r="D1" s="51" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="17.5" thickBot="1">
+      <c r="A2" s="52">
+        <v>2001</v>
+      </c>
+      <c r="B2" s="52" t="s">
+        <v>147</v>
+      </c>
+      <c r="C2" s="52" t="s">
+        <v>148</v>
+      </c>
+      <c r="D2" s="52"/>
+    </row>
+    <row r="3" spans="1:4" ht="17.5" thickBot="1">
+      <c r="A3" s="53">
+        <v>2002</v>
+      </c>
+      <c r="B3" s="53" t="s">
+        <v>149</v>
+      </c>
+      <c r="C3" s="53" t="s">
+        <v>150</v>
+      </c>
+      <c r="D3" s="53" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="17.5" thickBot="1">
+      <c r="A4" s="52">
+        <v>2003</v>
+      </c>
+      <c r="B4" s="52" t="s">
+        <v>152</v>
+      </c>
+      <c r="C4" s="52" t="s">
+        <v>153</v>
+      </c>
+      <c r="D4" s="52"/>
+    </row>
+    <row r="5" spans="1:4" ht="17.5" thickBot="1">
+      <c r="A5" s="53">
+        <v>2004</v>
+      </c>
+      <c r="B5" s="53" t="s">
+        <v>154</v>
+      </c>
+      <c r="C5" s="53" t="s">
+        <v>155</v>
+      </c>
+      <c r="D5" s="53"/>
+    </row>
+    <row r="6" spans="1:4" ht="17.5" thickBot="1">
+      <c r="A6" s="52">
+        <v>2005</v>
+      </c>
+      <c r="B6" s="52" t="s">
+        <v>156</v>
+      </c>
+      <c r="C6" s="52" t="s">
+        <v>157</v>
+      </c>
+      <c r="D6" s="52"/>
+    </row>
+    <row r="7" spans="1:4" ht="17.5" thickBot="1">
+      <c r="A7" s="53">
+        <v>2006</v>
+      </c>
+      <c r="B7" s="53" t="s">
+        <v>158</v>
+      </c>
+      <c r="C7" s="53" t="s">
+        <v>159</v>
+      </c>
+      <c r="D7" s="53" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="17.5" thickBot="1">
+      <c r="A8" s="52">
+        <v>2007</v>
+      </c>
+      <c r="B8" s="52" t="s">
+        <v>161</v>
+      </c>
+      <c r="C8" s="52" t="s">
+        <v>162</v>
+      </c>
+      <c r="D8" s="52" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="17.5" thickBot="1">
+      <c r="A9" s="53">
+        <v>2008</v>
+      </c>
+      <c r="B9" s="53" t="s">
+        <v>164</v>
+      </c>
+      <c r="C9" s="53" t="s">
+        <v>165</v>
+      </c>
+      <c r="D9" s="53"/>
+    </row>
+    <row r="10" spans="1:4" ht="17.5" thickBot="1">
+      <c r="A10" s="52">
+        <v>2009</v>
+      </c>
+      <c r="B10" s="52" t="s">
+        <v>166</v>
+      </c>
+      <c r="C10" s="52" t="s">
+        <v>167</v>
+      </c>
+      <c r="D10" s="52"/>
+    </row>
+    <row r="11" spans="1:4" ht="17.5" thickBot="1">
+      <c r="A11" s="53">
+        <v>2010</v>
+      </c>
+      <c r="B11" s="53" t="s">
+        <v>168</v>
+      </c>
+      <c r="C11" s="53" t="s">
+        <v>169</v>
+      </c>
+      <c r="D11" s="53" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="17.5" thickBot="1">
+      <c r="A12" s="52">
+        <v>2011</v>
+      </c>
+      <c r="B12" s="52" t="s">
+        <v>171</v>
+      </c>
+      <c r="C12" s="52" t="s">
+        <v>172</v>
+      </c>
+      <c r="D12" s="52"/>
+    </row>
+    <row r="13" spans="1:4" ht="17.5" thickBot="1">
+      <c r="A13" s="53">
+        <v>2012</v>
+      </c>
+      <c r="B13" s="53" t="s">
+        <v>173</v>
+      </c>
+      <c r="C13" s="53" t="s">
+        <v>174</v>
+      </c>
+      <c r="D13" s="53" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="17.5" thickBot="1">
+      <c r="A14" s="52">
+        <v>2013</v>
+      </c>
+      <c r="B14" s="52" t="s">
+        <v>176</v>
+      </c>
+      <c r="C14" s="52" t="s">
+        <v>177</v>
+      </c>
+      <c r="D14" s="52" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="17.5" thickBot="1">
+      <c r="A15" s="53">
+        <v>2014</v>
+      </c>
+      <c r="B15" s="53" t="s">
+        <v>179</v>
+      </c>
+      <c r="C15" s="53" t="s">
+        <v>177</v>
+      </c>
+      <c r="D15" s="53" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="17.5" thickBot="1">
+      <c r="A16" s="52">
+        <v>2015</v>
+      </c>
+      <c r="B16" s="52" t="s">
+        <v>181</v>
+      </c>
+      <c r="C16" s="52" t="s">
+        <v>177</v>
+      </c>
+      <c r="D16" s="52"/>
+    </row>
+    <row r="17" spans="1:4" ht="17.5" thickBot="1">
+      <c r="A17" s="53">
+        <v>2016</v>
+      </c>
+      <c r="B17" s="53" t="s">
+        <v>182</v>
+      </c>
+      <c r="C17" s="53" t="s">
+        <v>177</v>
+      </c>
+      <c r="D17" s="53" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="17.5" thickBot="1">
+      <c r="A18" s="52">
+        <v>2017</v>
+      </c>
+      <c r="B18" s="52" t="s">
+        <v>184</v>
+      </c>
+      <c r="C18" s="52" t="s">
+        <v>185</v>
+      </c>
+      <c r="D18" s="52" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="17.5" thickBot="1">
+      <c r="A19" s="53">
+        <v>2018</v>
+      </c>
+      <c r="B19" s="53" t="s">
+        <v>187</v>
+      </c>
+      <c r="C19" s="53" t="s">
+        <v>188</v>
+      </c>
+      <c r="D19" s="53"/>
+    </row>
+    <row r="20" spans="1:4" ht="17.5" thickBot="1">
+      <c r="A20" s="52">
+        <v>2019</v>
+      </c>
+      <c r="B20" s="52" t="s">
+        <v>189</v>
+      </c>
+      <c r="C20" s="52" t="s">
+        <v>190</v>
+      </c>
+      <c r="D20" s="52" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="17.5" thickBot="1">
+      <c r="A21" s="54">
+        <v>2020</v>
+      </c>
+      <c r="B21" s="54" t="s">
+        <v>192</v>
+      </c>
+      <c r="C21" s="54" t="s">
+        <v>193</v>
+      </c>
+      <c r="D21" s="54" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="17.5" thickTop="1"/>
+  </sheetData>
+  <phoneticPr fontId="4" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8F5942E8-E162-40EF-B993-3BAE903B1423}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="17"/>
+  <sheetData/>
+  <phoneticPr fontId="4" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B4A86FF2-E2FF-4B55-A0A8-4394346292FD}">
+  <dimension ref="B1:H15"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:H1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="17"/>
+  <cols>
+    <col min="2" max="2" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="72.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.4140625" customWidth="1"/>
+    <col min="6" max="6" width="9.1640625" customWidth="1"/>
+    <col min="7" max="7" width="9" customWidth="1"/>
+    <col min="8" max="8" width="12.58203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:8">
+      <c r="B1" s="40" t="s">
+        <v>79</v>
+      </c>
+      <c r="C1" s="40" t="s">
+        <v>80</v>
+      </c>
+      <c r="D1" s="40" t="s">
+        <v>86</v>
+      </c>
+      <c r="E1" s="40" t="s">
+        <v>85</v>
+      </c>
+      <c r="F1" s="40" t="s">
+        <v>87</v>
+      </c>
+      <c r="G1" s="40" t="s">
+        <v>72</v>
+      </c>
+      <c r="H1" s="40" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="2" spans="2:8">
+      <c r="B2" t="s">
+        <v>104</v>
+      </c>
+      <c r="C2" t="s">
+        <v>116</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="2:8">
+      <c r="B3" t="s">
+        <v>120</v>
+      </c>
+      <c r="C3" t="s">
+        <v>119</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="2:8">
+      <c r="B4" t="s">
+        <v>117</v>
+      </c>
+      <c r="C4" t="s">
+        <v>105</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="2:8">
+      <c r="B5" t="s">
+        <v>106</v>
+      </c>
+      <c r="C5" t="s">
+        <v>115</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="2:8">
+      <c r="B6" t="s">
+        <v>107</v>
+      </c>
+      <c r="C6" t="s">
+        <v>113</v>
+      </c>
+      <c r="D6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="2:8">
+      <c r="B7" t="s">
+        <v>109</v>
+      </c>
+      <c r="C7" t="s">
+        <v>110</v>
+      </c>
+      <c r="D7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="2:8">
+      <c r="B8" t="s">
+        <v>111</v>
+      </c>
+      <c r="C8" t="s">
+        <v>112</v>
+      </c>
+      <c r="D8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="2:8">
+      <c r="B9" t="s">
+        <v>114</v>
+      </c>
+      <c r="C9" t="s">
+        <v>108</v>
+      </c>
+      <c r="D9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="2:8">
+      <c r="C10" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="14" spans="2:8">
+      <c r="B14" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="15" spans="2:8">
+      <c r="B15" s="46" t="s">
+        <v>122</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="4" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="B15" r:id="rId1" xr:uid="{047EF97C-9105-44B3-9BB4-9F807CC5AA0C}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D873622-2459-4AA0-832D-ED8435E8D5B5}">
+  <dimension ref="A1:G13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="17"/>
+  <cols>
+    <col min="1" max="1" width="13.83203125" customWidth="1"/>
+    <col min="2" max="2" width="45.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="10.58203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7">
+      <c r="A1" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="A3" s="40" t="s">
+        <v>79</v>
+      </c>
+      <c r="B3" s="40" t="s">
+        <v>80</v>
+      </c>
+      <c r="C3" s="40" t="s">
+        <v>86</v>
+      </c>
+      <c r="D3" s="40" t="s">
+        <v>85</v>
+      </c>
+      <c r="E3" s="40" t="s">
+        <v>87</v>
+      </c>
+      <c r="F3" s="40" t="s">
+        <v>72</v>
+      </c>
+      <c r="G3" s="40" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="A4" s="19" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" t="s">
+        <v>124</v>
+      </c>
+      <c r="C4" s="19">
+        <v>2</v>
+      </c>
+      <c r="D4" s="34">
+        <v>2100000</v>
+      </c>
+      <c r="E4" s="35">
+        <f>C4*D4</f>
+        <v>4200000</v>
+      </c>
+      <c r="F4" s="36">
+        <f>E4/$E$13</f>
+        <v>0.71230748618208273</v>
+      </c>
+      <c r="G4" s="36">
+        <f>F4</f>
+        <v>0.71230748618208273</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="A5" s="19" t="s">
+        <v>92</v>
+      </c>
+      <c r="B5" t="s">
+        <v>132</v>
+      </c>
+      <c r="C5" s="19">
+        <v>1</v>
+      </c>
+      <c r="D5" s="34">
+        <v>450980</v>
+      </c>
+      <c r="E5" s="35">
+        <f>C5*D5</f>
+        <v>450980</v>
+      </c>
+      <c r="F5" s="36">
+        <f t="shared" ref="F5:F12" si="0">E5/$E$13</f>
+        <v>7.6484864313903736E-2</v>
+      </c>
+      <c r="G5" s="36">
+        <f>G4+F5</f>
+        <v>0.78879235049598651</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
+      <c r="A6" s="19" t="s">
+        <v>93</v>
+      </c>
+      <c r="B6" t="s">
+        <v>133</v>
+      </c>
+      <c r="C6" s="19">
+        <v>1</v>
+      </c>
+      <c r="D6" s="34">
+        <v>340000</v>
+      </c>
+      <c r="E6" s="35">
+        <f>C6*D6</f>
+        <v>340000</v>
+      </c>
+      <c r="F6" s="36">
+        <f t="shared" si="0"/>
+        <v>5.7662986976644792E-2</v>
+      </c>
+      <c r="G6" s="36">
+        <f t="shared" ref="G6:G12" si="1">G5+F6</f>
+        <v>0.84645533747263135</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
+      <c r="A7" s="19" t="s">
+        <v>125</v>
+      </c>
+      <c r="B7" t="s">
+        <v>134</v>
+      </c>
+      <c r="C7" s="19">
+        <v>2</v>
+      </c>
+      <c r="D7" s="34">
+        <v>148000</v>
+      </c>
+      <c r="E7" s="35">
+        <f>C7*D7</f>
+        <v>296000</v>
+      </c>
+      <c r="F7" s="36">
+        <f t="shared" si="0"/>
+        <v>5.0200718073784879E-2</v>
+      </c>
+      <c r="G7" s="36">
+        <f t="shared" si="1"/>
+        <v>0.89665605554641625</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="A8" s="47" t="s">
+        <v>95</v>
+      </c>
+      <c r="B8" s="47" t="s">
+        <v>83</v>
+      </c>
+      <c r="C8" s="47">
+        <v>1</v>
+      </c>
+      <c r="D8" s="48">
+        <v>240000</v>
+      </c>
+      <c r="E8" s="49">
+        <f>D8*C8</f>
+        <v>240000</v>
+      </c>
+      <c r="F8" s="36">
+        <f t="shared" si="0"/>
+        <v>4.0703284924690442E-2</v>
+      </c>
+      <c r="G8" s="36">
+        <f t="shared" si="1"/>
+        <v>0.93735934047110669</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
+      <c r="A9" s="19" t="s">
+        <v>94</v>
+      </c>
+      <c r="B9" t="s">
+        <v>126</v>
+      </c>
+      <c r="C9" s="19">
+        <v>1</v>
+      </c>
+      <c r="D9" s="34">
+        <v>150000</v>
+      </c>
+      <c r="E9" s="35">
+        <f>C9*D9</f>
+        <v>150000</v>
+      </c>
+      <c r="F9" s="36">
+        <f t="shared" si="0"/>
+        <v>2.5439553077931526E-2</v>
+      </c>
+      <c r="G9" s="36">
+        <f t="shared" si="1"/>
+        <v>0.96279889354903825</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7">
+      <c r="A10" s="19" t="s">
+        <v>98</v>
+      </c>
+      <c r="B10" t="s">
+        <v>131</v>
+      </c>
+      <c r="C10" s="19">
+        <v>1</v>
+      </c>
+      <c r="D10" s="34">
+        <v>120000</v>
+      </c>
+      <c r="E10" s="35">
+        <f>C10*D10</f>
+        <v>120000</v>
+      </c>
+      <c r="F10" s="36">
+        <f t="shared" si="0"/>
+        <v>2.0351642462345221E-2</v>
+      </c>
+      <c r="G10" s="36">
+        <f t="shared" si="1"/>
+        <v>0.98315053601138347</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7">
+      <c r="A11" s="19" t="s">
+        <v>127</v>
+      </c>
+      <c r="B11" t="s">
+        <v>128</v>
+      </c>
+      <c r="C11" s="19">
+        <v>1</v>
+      </c>
+      <c r="D11" s="34">
+        <v>52350</v>
+      </c>
+      <c r="E11" s="35">
+        <f>C11*D11</f>
+        <v>52350</v>
+      </c>
+      <c r="F11" s="36">
+        <f t="shared" si="0"/>
+        <v>8.8784040241981031E-3</v>
+      </c>
+      <c r="G11" s="36">
+        <f t="shared" si="1"/>
+        <v>0.99202894003558162</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7">
+      <c r="A12" s="41" t="s">
+        <v>129</v>
+      </c>
+      <c r="B12" s="37" t="s">
+        <v>130</v>
+      </c>
+      <c r="C12" s="41">
+        <v>1</v>
+      </c>
+      <c r="D12" s="38">
+        <v>47000</v>
+      </c>
+      <c r="E12" s="39">
+        <f>C12*D12</f>
+        <v>47000</v>
+      </c>
+      <c r="F12" s="36">
+        <f t="shared" si="0"/>
+        <v>7.9710599644185458E-3</v>
+      </c>
+      <c r="G12" s="36">
+        <f t="shared" si="1"/>
+        <v>1.0000000000000002</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7">
+      <c r="E13" s="35">
+        <f>SUM(E4:E12)</f>
+        <v>5896330</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A4:G12">
+    <sortCondition descending="1" ref="E4:E12"/>
+  </sortState>
+  <phoneticPr fontId="4" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{87DDC824-1885-4BF6-A627-81B33414A371}">
+  <dimension ref="A1:G13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="17"/>
+  <cols>
+    <col min="1" max="1" width="15.25" customWidth="1"/>
+    <col min="2" max="2" width="45.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="10.58203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6.08203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7">
+      <c r="A1" s="46" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="A3" s="40" t="s">
+        <v>79</v>
+      </c>
+      <c r="B3" s="40" t="s">
+        <v>80</v>
+      </c>
+      <c r="C3" s="40" t="s">
+        <v>86</v>
+      </c>
+      <c r="D3" s="40" t="s">
+        <v>85</v>
+      </c>
+      <c r="E3" s="40" t="s">
+        <v>87</v>
+      </c>
+      <c r="F3" s="40" t="s">
+        <v>72</v>
+      </c>
+      <c r="G3" s="40" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="A4" s="19" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" s="50" t="s">
+        <v>140</v>
+      </c>
+      <c r="C4" s="19">
+        <v>2</v>
+      </c>
+      <c r="D4" s="33">
+        <v>2000000</v>
+      </c>
+      <c r="E4" s="35">
+        <f>C4*D4</f>
+        <v>4000000</v>
+      </c>
+      <c r="F4" s="36">
+        <f>E4/$E$13</f>
+        <v>0.47571759025254656</v>
+      </c>
+      <c r="G4" s="36">
+        <f>F4</f>
+        <v>0.47571759025254656</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="A5" s="19" t="s">
+        <v>92</v>
+      </c>
+      <c r="B5" t="s">
+        <v>136</v>
+      </c>
+      <c r="C5" s="19">
+        <v>1</v>
+      </c>
+      <c r="D5" s="33">
+        <v>1599000</v>
+      </c>
+      <c r="E5" s="35">
+        <f>C5*D5</f>
+        <v>1599000</v>
+      </c>
+      <c r="F5" s="36">
+        <f t="shared" ref="F5:F12" si="0">E5/$E$13</f>
+        <v>0.19016810670345549</v>
+      </c>
+      <c r="G5" s="36">
+        <f>G4+F5</f>
+        <v>0.66588569695600208</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
+      <c r="A6" s="19" t="s">
+        <v>93</v>
+      </c>
+      <c r="B6" t="s">
+        <v>137</v>
+      </c>
+      <c r="C6" s="19">
+        <v>1</v>
+      </c>
+      <c r="D6" s="34">
+        <v>1390000</v>
+      </c>
+      <c r="E6" s="35">
+        <f>C6*D6</f>
+        <v>1390000</v>
+      </c>
+      <c r="F6" s="36">
+        <f t="shared" si="0"/>
+        <v>0.16531186261275993</v>
+      </c>
+      <c r="G6" s="36">
+        <f t="shared" ref="G6:G12" si="1">G5+F6</f>
+        <v>0.83119755956876196</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
+      <c r="A7" s="19" t="s">
+        <v>125</v>
+      </c>
+      <c r="B7" t="s">
+        <v>139</v>
+      </c>
+      <c r="C7" s="19">
+        <v>1</v>
+      </c>
+      <c r="D7" s="34">
+        <v>291000</v>
+      </c>
+      <c r="E7" s="35">
+        <f>C7*D7</f>
+        <v>291000</v>
+      </c>
+      <c r="F7" s="36">
+        <f t="shared" si="0"/>
+        <v>3.4608454690872766E-2</v>
+      </c>
+      <c r="G7" s="36">
+        <f t="shared" si="1"/>
+        <v>0.86580601425963477</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="A8" s="47" t="s">
+        <v>95</v>
+      </c>
+      <c r="B8" s="47" t="s">
+        <v>138</v>
+      </c>
+      <c r="C8" s="47">
+        <v>2</v>
+      </c>
+      <c r="D8" s="48">
+        <v>150000</v>
+      </c>
+      <c r="E8" s="49">
+        <f>D8*C8</f>
+        <v>300000</v>
+      </c>
+      <c r="F8" s="36">
+        <f t="shared" si="0"/>
+        <v>3.5678819268940995E-2</v>
+      </c>
+      <c r="G8" s="36">
+        <f t="shared" si="1"/>
+        <v>0.90148483352857578</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
+      <c r="A9" s="19" t="s">
+        <v>94</v>
+      </c>
+      <c r="B9" t="s">
+        <v>141</v>
+      </c>
+      <c r="C9" s="19">
+        <v>1</v>
+      </c>
+      <c r="D9" s="34">
+        <v>609000</v>
+      </c>
+      <c r="E9" s="35">
+        <f>C9*D9</f>
+        <v>609000</v>
+      </c>
+      <c r="F9" s="36">
+        <f t="shared" si="0"/>
+        <v>7.2428003115950212E-2</v>
+      </c>
+      <c r="G9" s="36">
+        <f t="shared" si="1"/>
+        <v>0.97391283664452599</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7">
+      <c r="A10" s="19" t="s">
+        <v>98</v>
+      </c>
+      <c r="C10" s="19">
+        <v>1</v>
+      </c>
+      <c r="D10" s="34">
+        <v>120000</v>
+      </c>
+      <c r="E10" s="35">
+        <f>C10*D10</f>
+        <v>120000</v>
+      </c>
+      <c r="F10" s="36">
+        <f t="shared" si="0"/>
+        <v>1.4271527707576398E-2</v>
+      </c>
+      <c r="G10" s="36">
+        <f t="shared" si="1"/>
+        <v>0.98818436435210244</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7">
+      <c r="A11" s="19" t="s">
+        <v>127</v>
+      </c>
+      <c r="C11" s="19">
+        <v>1</v>
+      </c>
+      <c r="D11" s="34">
+        <v>52350</v>
+      </c>
+      <c r="E11" s="35">
+        <f>C11*D11</f>
+        <v>52350</v>
+      </c>
+      <c r="F11" s="36">
+        <f t="shared" si="0"/>
+        <v>6.2259539624302035E-3</v>
+      </c>
+      <c r="G11" s="36">
+        <f t="shared" si="1"/>
+        <v>0.99441031831453264</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7">
+      <c r="A12" s="41" t="s">
+        <v>129</v>
+      </c>
+      <c r="B12" s="37"/>
+      <c r="C12" s="41">
+        <v>1</v>
+      </c>
+      <c r="D12" s="38">
+        <v>47000</v>
+      </c>
+      <c r="E12" s="39">
+        <f>C12*D12</f>
+        <v>47000</v>
+      </c>
+      <c r="F12" s="36">
+        <f t="shared" si="0"/>
+        <v>5.5896816854674224E-3</v>
+      </c>
+      <c r="G12" s="36">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7">
+      <c r="E13" s="35">
+        <f>SUM(E4:E12)</f>
+        <v>8408350</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="4" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="A1" r:id="rId1" xr:uid="{8BAE8E4D-4026-4E85-8F09-741BCE60DA1C}"/>
+    <hyperlink ref="D4" r:id="rId2" display="http://prod.danawa.com/info/?pcode=10142334&amp;keyword=i9+10980XE&amp;cate=113973" xr:uid="{B9CC7658-C188-42EB-B4B4-60E03177D57D}"/>
+    <hyperlink ref="D5" r:id="rId3" display="http://prod.danawa.com/info/?pcode=10142334&amp;keyword=i9+10980XE&amp;cate=113973" xr:uid="{8A3C165F-A548-4D62-812F-FA0BE290A0D5}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId4"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AC833C15-AE3B-4F6A-8335-1E95E1B4E9D7}">
   <dimension ref="A1:G39"/>
   <sheetViews>
@@ -1610,7 +3567,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{245DD18F-81E4-4B96-A4CC-9B65DF710EEE}">
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1"/>
@@ -1632,7 +3589,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A840B13-1320-49FC-8A85-B22CFFBD28DD}">
   <dimension ref="A2:A3"/>
   <sheetViews>
@@ -1658,11 +3615,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB16F9D2-96AB-4E96-A7E9-4401830552B5}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
@@ -1677,4 +3634,907 @@
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{948F9106-E4C7-417F-827C-0BD8E2D3CBDC}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="17"/>
+  <sheetData/>
+  <phoneticPr fontId="4" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{23C6837C-8CA7-45CE-A9B3-0462460F9893}">
+  <dimension ref="A1:I11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D11" sqref="C11:D11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.5"/>
+  <cols>
+    <col min="1" max="1" width="7.1640625" style="20" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.1640625" style="20" customWidth="1"/>
+    <col min="3" max="3" width="7.1640625" style="20" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="40" style="20" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="5.58203125" style="20" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11" style="20" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.75" style="20" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="6.4140625" style="20" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.33203125" style="20" bestFit="1" customWidth="1"/>
+    <col min="10" max="16384" width="8.6640625" style="20"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" ht="17">
+      <c r="A1" s="30" t="s">
+        <v>73</v>
+      </c>
+      <c r="B1" s="30" t="s">
+        <v>195</v>
+      </c>
+      <c r="C1" s="30" t="s">
+        <v>49</v>
+      </c>
+      <c r="D1" s="31" t="s">
+        <v>50</v>
+      </c>
+      <c r="E1" s="31" t="s">
+        <v>51</v>
+      </c>
+      <c r="F1" s="31" t="s">
+        <v>67</v>
+      </c>
+      <c r="G1" s="31" t="s">
+        <v>68</v>
+      </c>
+      <c r="H1" s="32" t="s">
+        <v>72</v>
+      </c>
+      <c r="I1" s="32" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="17" customHeight="1">
+      <c r="A2" s="21">
+        <v>1</v>
+      </c>
+      <c r="B2" s="21" t="s">
+        <v>196</v>
+      </c>
+      <c r="C2" s="21" t="s">
+        <v>60</v>
+      </c>
+      <c r="D2" s="22" t="s">
+        <v>69</v>
+      </c>
+      <c r="E2" s="23">
+        <v>2</v>
+      </c>
+      <c r="F2" s="24">
+        <v>2000000</v>
+      </c>
+      <c r="G2" s="24">
+        <f t="shared" ref="G2:G10" si="0">E2*F2</f>
+        <v>4000000</v>
+      </c>
+      <c r="H2" s="25">
+        <f t="shared" ref="H2:H10" si="1">G2/$G$11</f>
+        <v>0.44198895027624308</v>
+      </c>
+      <c r="I2" s="25">
+        <f>H2</f>
+        <v>0.44198895027624308</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="17" customHeight="1">
+      <c r="A3" s="21">
+        <v>2</v>
+      </c>
+      <c r="B3" s="21" t="s">
+        <v>196</v>
+      </c>
+      <c r="C3" s="21" t="s">
+        <v>54</v>
+      </c>
+      <c r="D3" s="22" t="s">
+        <v>55</v>
+      </c>
+      <c r="E3" s="23">
+        <v>1</v>
+      </c>
+      <c r="F3" s="24">
+        <v>1500000</v>
+      </c>
+      <c r="G3" s="24">
+        <f t="shared" si="0"/>
+        <v>1500000</v>
+      </c>
+      <c r="H3" s="25">
+        <f t="shared" si="1"/>
+        <v>0.16574585635359115</v>
+      </c>
+      <c r="I3" s="25">
+        <f>I2+H3</f>
+        <v>0.60773480662983426</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="17" customHeight="1">
+      <c r="A4" s="21">
+        <v>3</v>
+      </c>
+      <c r="B4" s="21" t="s">
+        <v>196</v>
+      </c>
+      <c r="C4" s="21" t="s">
+        <v>58</v>
+      </c>
+      <c r="D4" s="22" t="s">
+        <v>70</v>
+      </c>
+      <c r="E4" s="23">
+        <v>8</v>
+      </c>
+      <c r="F4" s="24">
+        <v>150000</v>
+      </c>
+      <c r="G4" s="24">
+        <f t="shared" si="0"/>
+        <v>1200000</v>
+      </c>
+      <c r="H4" s="25">
+        <f t="shared" si="1"/>
+        <v>0.13259668508287292</v>
+      </c>
+      <c r="I4" s="25">
+        <f t="shared" ref="I4:I10" si="2">I3+H4</f>
+        <v>0.74033149171270718</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="17" customHeight="1">
+      <c r="A5" s="21">
+        <v>4</v>
+      </c>
+      <c r="B5" s="21" t="s">
+        <v>196</v>
+      </c>
+      <c r="C5" s="21" t="s">
+        <v>59</v>
+      </c>
+      <c r="D5" s="22" t="s">
+        <v>142</v>
+      </c>
+      <c r="E5" s="23">
+        <v>1</v>
+      </c>
+      <c r="F5" s="26">
+        <v>1000000</v>
+      </c>
+      <c r="G5" s="24">
+        <f t="shared" si="0"/>
+        <v>1000000</v>
+      </c>
+      <c r="H5" s="25">
+        <f t="shared" si="1"/>
+        <v>0.11049723756906077</v>
+      </c>
+      <c r="I5" s="25">
+        <f t="shared" si="2"/>
+        <v>0.850828729281768</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="17" customHeight="1">
+      <c r="A6" s="21">
+        <v>5</v>
+      </c>
+      <c r="B6" s="21" t="s">
+        <v>196</v>
+      </c>
+      <c r="C6" s="21" t="s">
+        <v>65</v>
+      </c>
+      <c r="D6" s="22" t="s">
+        <v>66</v>
+      </c>
+      <c r="E6" s="23">
+        <v>1</v>
+      </c>
+      <c r="F6" s="24">
+        <v>500000</v>
+      </c>
+      <c r="G6" s="24">
+        <f t="shared" si="0"/>
+        <v>500000</v>
+      </c>
+      <c r="H6" s="25">
+        <f t="shared" si="1"/>
+        <v>5.5248618784530384E-2</v>
+      </c>
+      <c r="I6" s="25">
+        <f t="shared" si="2"/>
+        <v>0.90607734806629836</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="17" customHeight="1">
+      <c r="A7" s="21">
+        <v>6</v>
+      </c>
+      <c r="B7" s="21" t="s">
+        <v>196</v>
+      </c>
+      <c r="C7" s="21" t="s">
+        <v>56</v>
+      </c>
+      <c r="D7" s="22" t="s">
+        <v>57</v>
+      </c>
+      <c r="E7" s="23">
+        <v>1</v>
+      </c>
+      <c r="F7" s="26">
+        <v>250000</v>
+      </c>
+      <c r="G7" s="24">
+        <f t="shared" si="0"/>
+        <v>250000</v>
+      </c>
+      <c r="H7" s="25">
+        <f t="shared" si="1"/>
+        <v>2.7624309392265192E-2</v>
+      </c>
+      <c r="I7" s="25">
+        <f t="shared" si="2"/>
+        <v>0.93370165745856359</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="17" customHeight="1">
+      <c r="A8" s="21">
+        <v>7</v>
+      </c>
+      <c r="B8" s="21" t="s">
+        <v>196</v>
+      </c>
+      <c r="C8" s="21" t="s">
+        <v>61</v>
+      </c>
+      <c r="D8" s="22" t="s">
+        <v>62</v>
+      </c>
+      <c r="E8" s="23">
+        <v>1</v>
+      </c>
+      <c r="F8" s="24">
+        <v>250000</v>
+      </c>
+      <c r="G8" s="24">
+        <f t="shared" si="0"/>
+        <v>250000</v>
+      </c>
+      <c r="H8" s="25">
+        <f t="shared" si="1"/>
+        <v>2.7624309392265192E-2</v>
+      </c>
+      <c r="I8" s="25">
+        <f t="shared" si="2"/>
+        <v>0.96132596685082883</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="17" customHeight="1">
+      <c r="A9" s="21">
+        <v>8</v>
+      </c>
+      <c r="B9" s="21" t="s">
+        <v>196</v>
+      </c>
+      <c r="C9" s="21" t="s">
+        <v>52</v>
+      </c>
+      <c r="D9" s="27" t="s">
+        <v>53</v>
+      </c>
+      <c r="E9" s="23">
+        <v>1</v>
+      </c>
+      <c r="F9" s="28">
+        <v>200000</v>
+      </c>
+      <c r="G9" s="24">
+        <f t="shared" si="0"/>
+        <v>200000</v>
+      </c>
+      <c r="H9" s="25">
+        <f t="shared" si="1"/>
+        <v>2.2099447513812154E-2</v>
+      </c>
+      <c r="I9" s="25">
+        <f t="shared" si="2"/>
+        <v>0.98342541436464104</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="17" customHeight="1">
+      <c r="A10" s="21">
+        <v>9</v>
+      </c>
+      <c r="B10" s="21" t="s">
+        <v>196</v>
+      </c>
+      <c r="C10" s="21" t="s">
+        <v>63</v>
+      </c>
+      <c r="D10" s="22" t="s">
+        <v>64</v>
+      </c>
+      <c r="E10" s="23">
+        <v>1</v>
+      </c>
+      <c r="F10" s="24">
+        <v>150000</v>
+      </c>
+      <c r="G10" s="24">
+        <f t="shared" si="0"/>
+        <v>150000</v>
+      </c>
+      <c r="H10" s="25">
+        <f t="shared" si="1"/>
+        <v>1.6574585635359115E-2</v>
+      </c>
+      <c r="I10" s="25">
+        <f t="shared" si="2"/>
+        <v>1.0000000000000002</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9">
+      <c r="G11" s="29">
+        <f>SUM(G2:G10)</f>
+        <v>9050000</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="C2:H10">
+    <sortCondition descending="1" ref="G2:G10"/>
+  </sortState>
+  <phoneticPr fontId="4" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{69D377AF-A61F-46F2-AA80-700D78678B17}">
+  <dimension ref="A1:G15"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A11" sqref="A11:G11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="17"/>
+  <cols>
+    <col min="1" max="1" width="16.08203125" customWidth="1"/>
+    <col min="2" max="2" width="41.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="10.58203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7">
+      <c r="A1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="A2" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="A3" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="A4" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="A5" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
+      <c r="A6" s="40" t="s">
+        <v>79</v>
+      </c>
+      <c r="B6" s="40" t="s">
+        <v>80</v>
+      </c>
+      <c r="C6" s="40" t="s">
+        <v>86</v>
+      </c>
+      <c r="D6" s="40" t="s">
+        <v>85</v>
+      </c>
+      <c r="E6" s="40" t="s">
+        <v>87</v>
+      </c>
+      <c r="F6" s="40" t="s">
+        <v>72</v>
+      </c>
+      <c r="G6" s="40" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
+      <c r="A7" s="41" t="s">
+        <v>91</v>
+      </c>
+      <c r="B7" s="41" t="s">
+        <v>84</v>
+      </c>
+      <c r="C7" s="41">
+        <v>2</v>
+      </c>
+      <c r="D7" s="42">
+        <v>2030000</v>
+      </c>
+      <c r="E7" s="43">
+        <f t="shared" ref="E7:E14" si="0">D7*C7</f>
+        <v>4060000</v>
+      </c>
+      <c r="F7" s="44">
+        <f t="shared" ref="F7:F14" si="1">E7/$E$15</f>
+        <v>0.61515710748885599</v>
+      </c>
+      <c r="G7" s="44">
+        <f>F7</f>
+        <v>0.61515710748885599</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="A8" s="41" t="s">
+        <v>92</v>
+      </c>
+      <c r="B8" s="41" t="s">
+        <v>81</v>
+      </c>
+      <c r="C8" s="41">
+        <v>1</v>
+      </c>
+      <c r="D8" s="42">
+        <v>780460</v>
+      </c>
+      <c r="E8" s="43">
+        <f t="shared" si="0"/>
+        <v>780460</v>
+      </c>
+      <c r="F8" s="44">
+        <f t="shared" si="1"/>
+        <v>0.11825259017506219</v>
+      </c>
+      <c r="G8" s="44">
+        <f>G7+F8</f>
+        <v>0.73340969766391817</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
+      <c r="A9" s="41" t="s">
+        <v>93</v>
+      </c>
+      <c r="B9" s="41" t="s">
+        <v>82</v>
+      </c>
+      <c r="C9" s="41">
+        <v>1</v>
+      </c>
+      <c r="D9" s="42">
+        <v>644000</v>
+      </c>
+      <c r="E9" s="43">
+        <f t="shared" si="0"/>
+        <v>644000</v>
+      </c>
+      <c r="F9" s="44">
+        <f t="shared" si="1"/>
+        <v>9.7576644636163362E-2</v>
+      </c>
+      <c r="G9" s="44">
+        <f t="shared" ref="G9:G14" si="2">G8+F9</f>
+        <v>0.8309863423000815</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7">
+      <c r="A10" s="41" t="s">
+        <v>94</v>
+      </c>
+      <c r="B10" s="41" t="s">
+        <v>89</v>
+      </c>
+      <c r="C10" s="41">
+        <v>1</v>
+      </c>
+      <c r="D10" s="42">
+        <v>530000</v>
+      </c>
+      <c r="E10" s="43">
+        <f t="shared" si="0"/>
+        <v>530000</v>
+      </c>
+      <c r="F10" s="44">
+        <f t="shared" si="1"/>
+        <v>8.0303760337215188E-2</v>
+      </c>
+      <c r="G10" s="44">
+        <f t="shared" si="2"/>
+        <v>0.91129010263729671</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7">
+      <c r="A11" s="41" t="s">
+        <v>95</v>
+      </c>
+      <c r="B11" s="41" t="s">
+        <v>83</v>
+      </c>
+      <c r="C11" s="41">
+        <v>1</v>
+      </c>
+      <c r="D11" s="42">
+        <v>240000</v>
+      </c>
+      <c r="E11" s="43">
+        <f t="shared" si="0"/>
+        <v>240000</v>
+      </c>
+      <c r="F11" s="44">
+        <f t="shared" si="1"/>
+        <v>3.636396694515405E-2</v>
+      </c>
+      <c r="G11" s="44">
+        <f t="shared" si="2"/>
+        <v>0.9476540695824508</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7">
+      <c r="A12" s="41" t="s">
+        <v>96</v>
+      </c>
+      <c r="B12" s="41" t="s">
+        <v>88</v>
+      </c>
+      <c r="C12" s="41">
+        <v>1</v>
+      </c>
+      <c r="D12" s="42">
+        <v>125480</v>
+      </c>
+      <c r="E12" s="43">
+        <f t="shared" si="0"/>
+        <v>125480</v>
+      </c>
+      <c r="F12" s="44">
+        <f t="shared" si="1"/>
+        <v>1.9012294051158042E-2</v>
+      </c>
+      <c r="G12" s="44">
+        <f t="shared" si="2"/>
+        <v>0.96666636363360881</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7">
+      <c r="A13" s="41" t="s">
+        <v>97</v>
+      </c>
+      <c r="B13" s="41" t="s">
+        <v>77</v>
+      </c>
+      <c r="C13" s="41">
+        <v>1</v>
+      </c>
+      <c r="D13" s="42">
+        <v>120000</v>
+      </c>
+      <c r="E13" s="43">
+        <f t="shared" si="0"/>
+        <v>120000</v>
+      </c>
+      <c r="F13" s="44">
+        <f t="shared" si="1"/>
+        <v>1.8181983472577025E-2</v>
+      </c>
+      <c r="G13" s="44">
+        <f t="shared" si="2"/>
+        <v>0.98484834710618585</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7">
+      <c r="A14" s="41" t="s">
+        <v>98</v>
+      </c>
+      <c r="B14" s="41" t="s">
+        <v>90</v>
+      </c>
+      <c r="C14" s="41">
+        <v>1</v>
+      </c>
+      <c r="D14" s="42">
+        <v>100000</v>
+      </c>
+      <c r="E14" s="43">
+        <f t="shared" si="0"/>
+        <v>100000</v>
+      </c>
+      <c r="F14" s="44">
+        <f t="shared" si="1"/>
+        <v>1.5151652893814186E-2</v>
+      </c>
+      <c r="G14" s="44">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7">
+      <c r="E15" s="35">
+        <f>SUM(E7:E14)</f>
+        <v>6599940</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A7:G14">
+    <sortCondition descending="1" ref="E7:E14"/>
+  </sortState>
+  <phoneticPr fontId="4" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{123DB921-81D0-46D6-8F37-7436046A6F9E}">
+  <dimension ref="A1:H9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="17"/>
+  <cols>
+    <col min="1" max="1" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="41.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="10.58203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8">
+      <c r="A1" s="40" t="s">
+        <v>79</v>
+      </c>
+      <c r="B1" s="40" t="s">
+        <v>80</v>
+      </c>
+      <c r="C1" s="40" t="s">
+        <v>86</v>
+      </c>
+      <c r="D1" s="40" t="s">
+        <v>85</v>
+      </c>
+      <c r="E1" s="40" t="s">
+        <v>87</v>
+      </c>
+      <c r="F1" s="40" t="s">
+        <v>72</v>
+      </c>
+      <c r="G1" s="40" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
+      <c r="A2" s="41" t="s">
+        <v>91</v>
+      </c>
+      <c r="B2" s="41" t="s">
+        <v>99</v>
+      </c>
+      <c r="C2" s="41">
+        <v>2</v>
+      </c>
+      <c r="D2" s="42">
+        <v>2030000</v>
+      </c>
+      <c r="E2" s="43">
+        <f t="shared" ref="E2:E9" si="0">D2*C2</f>
+        <v>4060000</v>
+      </c>
+      <c r="F2" s="44" t="e">
+        <f t="shared" ref="F2:F9" si="1">E2/$E$15</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G2" s="44" t="e">
+        <f>F2</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
+      <c r="A3" s="41" t="s">
+        <v>92</v>
+      </c>
+      <c r="B3" s="41" t="s">
+        <v>101</v>
+      </c>
+      <c r="C3" s="41">
+        <v>1</v>
+      </c>
+      <c r="D3" s="42">
+        <v>700000</v>
+      </c>
+      <c r="E3" s="43">
+        <f t="shared" si="0"/>
+        <v>700000</v>
+      </c>
+      <c r="F3" s="44" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G3" s="44" t="e">
+        <f>G2+F3</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H3" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
+      <c r="A4" s="41" t="s">
+        <v>93</v>
+      </c>
+      <c r="B4" s="41"/>
+      <c r="C4" s="41">
+        <v>1</v>
+      </c>
+      <c r="D4" s="42">
+        <v>644000</v>
+      </c>
+      <c r="E4" s="43">
+        <f t="shared" si="0"/>
+        <v>644000</v>
+      </c>
+      <c r="F4" s="44" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G4" s="44" t="e">
+        <f t="shared" ref="G4:G9" si="2">G3+F4</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
+      <c r="A5" s="41" t="s">
+        <v>94</v>
+      </c>
+      <c r="B5" s="45" t="s">
+        <v>103</v>
+      </c>
+      <c r="C5" s="41">
+        <v>1</v>
+      </c>
+      <c r="D5" s="42">
+        <v>400000</v>
+      </c>
+      <c r="E5" s="43">
+        <f t="shared" si="0"/>
+        <v>400000</v>
+      </c>
+      <c r="F5" s="44" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G5" s="44" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
+      <c r="A6" s="41" t="s">
+        <v>95</v>
+      </c>
+      <c r="B6" s="41" t="s">
+        <v>100</v>
+      </c>
+      <c r="C6" s="41">
+        <v>2</v>
+      </c>
+      <c r="D6" s="42">
+        <v>240000</v>
+      </c>
+      <c r="E6" s="43">
+        <f t="shared" si="0"/>
+        <v>480000</v>
+      </c>
+      <c r="F6" s="44" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G6" s="44" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8">
+      <c r="A7" s="41" t="s">
+        <v>96</v>
+      </c>
+      <c r="B7" s="41"/>
+      <c r="C7" s="41">
+        <v>1</v>
+      </c>
+      <c r="D7" s="42">
+        <v>125480</v>
+      </c>
+      <c r="E7" s="43">
+        <f t="shared" si="0"/>
+        <v>125480</v>
+      </c>
+      <c r="F7" s="44" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G7" s="44" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8">
+      <c r="A8" s="41" t="s">
+        <v>97</v>
+      </c>
+      <c r="B8" s="41"/>
+      <c r="C8" s="41">
+        <v>1</v>
+      </c>
+      <c r="D8" s="42">
+        <v>120000</v>
+      </c>
+      <c r="E8" s="43">
+        <f t="shared" si="0"/>
+        <v>120000</v>
+      </c>
+      <c r="F8" s="44" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G8" s="44" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8">
+      <c r="A9" s="41" t="s">
+        <v>98</v>
+      </c>
+      <c r="B9" s="41"/>
+      <c r="C9" s="41">
+        <v>1</v>
+      </c>
+      <c r="D9" s="42">
+        <v>100000</v>
+      </c>
+      <c r="E9" s="43">
+        <f t="shared" si="0"/>
+        <v>100000</v>
+      </c>
+      <c r="F9" s="44" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G9" s="44" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="4" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>